<commit_message>
making sourcing universal, almost
</commit_message>
<xml_diff>
--- a/apple_finrep/output.xlsx
+++ b/apple_finrep/output.xlsx
@@ -31,199 +31,199 @@
     <t>built_in_total</t>
   </si>
   <si>
+    <t>87811004_1121_AU</t>
+  </si>
+  <si>
+    <t>87811004_1121_BG</t>
+  </si>
+  <si>
+    <t>87811004_1121_BR</t>
+  </si>
+  <si>
+    <t>87811004_1121_CA</t>
+  </si>
+  <si>
+    <t>87811004_1121_CH</t>
+  </si>
+  <si>
+    <t>87811004_1121_CL</t>
+  </si>
+  <si>
+    <t>87811004_1121_CO</t>
+  </si>
+  <si>
+    <t>87811004_1121_CZ</t>
+  </si>
+  <si>
+    <t>87811004_1121_DK</t>
+  </si>
+  <si>
+    <t>87811004_1121_EU</t>
+  </si>
+  <si>
+    <t>87811004_1121_GB</t>
+  </si>
+  <si>
+    <t>87811004_1121_HU</t>
+  </si>
+  <si>
+    <t>87811004_1121_JP</t>
+  </si>
+  <si>
+    <t>87811004_1121_LL</t>
+  </si>
+  <si>
     <t>87811004_1121_MX</t>
   </si>
   <si>
-    <t>87811004_1121_BR</t>
-  </si>
-  <si>
-    <t>87811004_1121_CA</t>
-  </si>
-  <si>
-    <t>87811004_1121_LL</t>
-  </si>
-  <si>
-    <t>87811004_1121_BG</t>
-  </si>
-  <si>
-    <t>87811004_1121_HU</t>
+    <t>87811004_1121_NO</t>
+  </si>
+  <si>
+    <t>87811004_1121_NZ</t>
   </si>
   <si>
     <t>87811004_1121_PE</t>
   </si>
   <si>
+    <t>87811004_1121_PL</t>
+  </si>
+  <si>
     <t>87811004_1121_RO</t>
   </si>
   <si>
-    <t>87811004_1121_EU</t>
-  </si>
-  <si>
-    <t>87811004_1121_PL</t>
-  </si>
-  <si>
-    <t>87811004_1121_DK</t>
-  </si>
-  <si>
-    <t>87811004_1121_GB</t>
-  </si>
-  <si>
     <t>87811004_1121_SE</t>
   </si>
   <si>
-    <t>87811004_1121_JP</t>
-  </si>
-  <si>
-    <t>87811004_1121_CO</t>
-  </si>
-  <si>
-    <t>87811004_1121_CL</t>
-  </si>
-  <si>
-    <t>87811004_1121_CZ</t>
-  </si>
-  <si>
     <t>87811004_1121_US</t>
   </si>
   <si>
-    <t>87811004_1121_CH</t>
-  </si>
-  <si>
-    <t>87811004_1121_NO</t>
-  </si>
-  <si>
-    <t>87811004_1121_NZ</t>
-  </si>
-  <si>
-    <t>87811004_1121_AU</t>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
   <si>
     <t>MXN</t>
   </si>
   <si>
-    <t>BRL</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>BGN</t>
-  </si>
-  <si>
-    <t>HUF</t>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>NZD</t>
   </si>
   <si>
     <t>PEN</t>
   </si>
   <si>
+    <t>PLN</t>
+  </si>
+  <si>
     <t>RON</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>DKK</t>
-  </si>
-  <si>
-    <t>GBP</t>
-  </si>
-  <si>
     <t>SEK</t>
   </si>
   <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>CZK</t>
-  </si>
-  <si>
-    <t>CHF</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>AUD</t>
+    <t>1617.46</t>
+  </si>
+  <si>
+    <t>16.04</t>
+  </si>
+  <si>
+    <t>440.44</t>
+  </si>
+  <si>
+    <t>1332.8</t>
+  </si>
+  <si>
+    <t>387.56</t>
+  </si>
+  <si>
+    <t>73248</t>
+  </si>
+  <si>
+    <t>347830</t>
+  </si>
+  <si>
+    <t>1718.21</t>
+  </si>
+  <si>
+    <t>440.16</t>
+  </si>
+  <si>
+    <t>3309.31</t>
+  </si>
+  <si>
+    <t>1309.43</t>
+  </si>
+  <si>
+    <t>1915878</t>
+  </si>
+  <si>
+    <t>7546</t>
+  </si>
+  <si>
+    <t>112</t>
   </si>
   <si>
     <t>7567.7</t>
   </si>
   <si>
-    <t>440.44</t>
-  </si>
-  <si>
-    <t>1332.8</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>16.04</t>
-  </si>
-  <si>
-    <t>1915878</t>
+    <t>655.2</t>
+  </si>
+  <si>
+    <t>147.6</t>
   </si>
   <si>
     <t>174.3</t>
   </si>
   <si>
+    <t>401.94</t>
+  </si>
+  <si>
     <t>9795.57</t>
   </si>
   <si>
-    <t>3309.31</t>
-  </si>
-  <si>
-    <t>401.94</t>
-  </si>
-  <si>
-    <t>440.16</t>
-  </si>
-  <si>
-    <t>1309.43</t>
-  </si>
-  <si>
     <t>919.87</t>
   </si>
   <si>
-    <t>7546</t>
-  </si>
-  <si>
-    <t>347830</t>
-  </si>
-  <si>
-    <t>73248</t>
-  </si>
-  <si>
-    <t>1718.21</t>
-  </si>
-  <si>
     <t>8030.4</t>
-  </si>
-  <si>
-    <t>387.56</t>
-  </si>
-  <si>
-    <t>655.2</t>
-  </si>
-  <si>
-    <t>147.6</t>
-  </si>
-  <si>
-    <t>1617.46</t>
   </si>
 </sst>
 </file>
@@ -623,13 +623,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>78</v>
+        <v>307</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2">
-        <v>7567.7</v>
+        <v>1617.46</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
@@ -640,13 +640,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2">
-        <v>440.44</v>
+        <v>16.04</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -657,13 +657,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>287</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>1332.8</v>
+        <v>440.44</v>
       </c>
       <c r="E4" t="s">
         <v>50</v>
@@ -674,13 +674,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>43</v>
+        <v>287</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>112</v>
+        <v>1332.8</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -691,13 +691,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
-        <v>16.04</v>
+        <v>387.56</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -708,13 +708,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>900</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="2">
-        <v>1915878</v>
+        <v>73248</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -725,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>174.3</v>
+        <v>347830</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -742,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>494</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="2">
-        <v>9795.57</v>
+        <v>1718.21</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
@@ -759,13 +759,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>746</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="2">
-        <v>3309.31</v>
+        <v>440.16</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -776,13 +776,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>42</v>
+        <v>746</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>401.94</v>
+        <v>3309.31</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -793,13 +793,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>22</v>
+        <v>400</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>440.16</v>
+        <v>1309.43</v>
       </c>
       <c r="E12" t="s">
         <v>58</v>
@@ -810,13 +810,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>400</v>
+        <v>900</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>1309.43</v>
+        <v>1915878</v>
       </c>
       <c r="E13" t="s">
         <v>59</v>
@@ -827,13 +827,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>919.87</v>
+        <v>7546</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
@@ -844,13 +844,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>7546</v>
+        <v>112</v>
       </c>
       <c r="E15" t="s">
         <v>61</v>
@@ -861,13 +861,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>347830</v>
+        <v>7567.7</v>
       </c>
       <c r="E16" t="s">
         <v>62</v>
@@ -878,13 +878,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="2">
-        <v>73248</v>
+        <v>655.2</v>
       </c>
       <c r="E17" t="s">
         <v>63</v>
@@ -895,13 +895,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="2">
-        <v>1718.21</v>
+        <v>147.6</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -912,13 +912,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>1415</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2">
-        <v>8030.4</v>
+        <v>174.3</v>
       </c>
       <c r="E19" t="s">
         <v>65</v>
@@ -929,13 +929,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2">
-        <v>387.56</v>
+        <v>401.94</v>
       </c>
       <c r="E20" t="s">
         <v>66</v>
@@ -946,13 +946,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>26</v>
+        <v>494</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2">
-        <v>655.2</v>
+        <v>9795.57</v>
       </c>
       <c r="E21" t="s">
         <v>67</v>
@@ -963,13 +963,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2">
-        <v>147.6</v>
+        <v>919.87</v>
       </c>
       <c r="E22" t="s">
         <v>68</v>
@@ -980,13 +980,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="2">
-        <v>307</v>
+        <v>1415</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D23" s="2">
-        <v>1617.46</v>
+        <v>8030.4</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
moved google files to store
</commit_message>
<xml_diff>
--- a/apple_finrep/output.xlsx
+++ b/apple_finrep/output.xlsx
@@ -31,199 +31,199 @@
     <t>built_in_total</t>
   </si>
   <si>
+    <t>87811004_1121_MX</t>
+  </si>
+  <si>
+    <t>87811004_1121_BR</t>
+  </si>
+  <si>
+    <t>87811004_1121_CA</t>
+  </si>
+  <si>
+    <t>87811004_1121_LL</t>
+  </si>
+  <si>
+    <t>87811004_1121_BG</t>
+  </si>
+  <si>
+    <t>87811004_1121_HU</t>
+  </si>
+  <si>
+    <t>87811004_1121_PE</t>
+  </si>
+  <si>
+    <t>87811004_1121_RO</t>
+  </si>
+  <si>
+    <t>87811004_1121_EU</t>
+  </si>
+  <si>
+    <t>87811004_1121_PL</t>
+  </si>
+  <si>
+    <t>87811004_1121_DK</t>
+  </si>
+  <si>
+    <t>87811004_1121_GB</t>
+  </si>
+  <si>
+    <t>87811004_1121_SE</t>
+  </si>
+  <si>
+    <t>87811004_1121_JP</t>
+  </si>
+  <si>
+    <t>87811004_1121_CO</t>
+  </si>
+  <si>
+    <t>87811004_1121_CL</t>
+  </si>
+  <si>
+    <t>87811004_1121_CZ</t>
+  </si>
+  <si>
+    <t>87811004_1121_US</t>
+  </si>
+  <si>
+    <t>87811004_1121_CH</t>
+  </si>
+  <si>
+    <t>87811004_1121_NO</t>
+  </si>
+  <si>
+    <t>87811004_1121_NZ</t>
+  </si>
+  <si>
     <t>87811004_1121_AU</t>
   </si>
   <si>
-    <t>87811004_1121_BG</t>
-  </si>
-  <si>
-    <t>87811004_1121_BR</t>
-  </si>
-  <si>
-    <t>87811004_1121_CA</t>
-  </si>
-  <si>
-    <t>87811004_1121_CH</t>
-  </si>
-  <si>
-    <t>87811004_1121_CL</t>
-  </si>
-  <si>
-    <t>87811004_1121_CO</t>
-  </si>
-  <si>
-    <t>87811004_1121_CZ</t>
-  </si>
-  <si>
-    <t>87811004_1121_DK</t>
-  </si>
-  <si>
-    <t>87811004_1121_EU</t>
-  </si>
-  <si>
-    <t>87811004_1121_GB</t>
-  </si>
-  <si>
-    <t>87811004_1121_HU</t>
-  </si>
-  <si>
-    <t>87811004_1121_JP</t>
-  </si>
-  <si>
-    <t>87811004_1121_LL</t>
-  </si>
-  <si>
-    <t>87811004_1121_MX</t>
-  </si>
-  <si>
-    <t>87811004_1121_NO</t>
-  </si>
-  <si>
-    <t>87811004_1121_NZ</t>
-  </si>
-  <si>
-    <t>87811004_1121_PE</t>
-  </si>
-  <si>
-    <t>87811004_1121_PL</t>
-  </si>
-  <si>
-    <t>87811004_1121_RO</t>
-  </si>
-  <si>
-    <t>87811004_1121_SE</t>
-  </si>
-  <si>
-    <t>87811004_1121_US</t>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>NZD</t>
   </si>
   <si>
     <t>AUD</t>
   </si>
   <si>
-    <t>BGN</t>
-  </si>
-  <si>
-    <t>BRL</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>CHF</t>
-  </si>
-  <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>CZK</t>
-  </si>
-  <si>
-    <t>DKK</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>GBP</t>
-  </si>
-  <si>
-    <t>HUF</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>MXN</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>PEN</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>RON</t>
-  </si>
-  <si>
-    <t>SEK</t>
+    <t>7567.7</t>
+  </si>
+  <si>
+    <t>440.44</t>
+  </si>
+  <si>
+    <t>1332.8</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>16.04</t>
+  </si>
+  <si>
+    <t>1915878</t>
+  </si>
+  <si>
+    <t>174.3</t>
+  </si>
+  <si>
+    <t>9795.57</t>
+  </si>
+  <si>
+    <t>3309.31</t>
+  </si>
+  <si>
+    <t>401.94</t>
+  </si>
+  <si>
+    <t>440.16</t>
+  </si>
+  <si>
+    <t>1309.43</t>
+  </si>
+  <si>
+    <t>919.87</t>
+  </si>
+  <si>
+    <t>7546</t>
+  </si>
+  <si>
+    <t>347830</t>
+  </si>
+  <si>
+    <t>73248</t>
+  </si>
+  <si>
+    <t>1718.21</t>
+  </si>
+  <si>
+    <t>8030.4</t>
+  </si>
+  <si>
+    <t>387.56</t>
+  </si>
+  <si>
+    <t>655.2</t>
+  </si>
+  <si>
+    <t>147.6</t>
   </si>
   <si>
     <t>1617.46</t>
-  </si>
-  <si>
-    <t>16.04</t>
-  </si>
-  <si>
-    <t>440.44</t>
-  </si>
-  <si>
-    <t>1332.8</t>
-  </si>
-  <si>
-    <t>387.56</t>
-  </si>
-  <si>
-    <t>73248</t>
-  </si>
-  <si>
-    <t>347830</t>
-  </si>
-  <si>
-    <t>1718.21</t>
-  </si>
-  <si>
-    <t>440.16</t>
-  </si>
-  <si>
-    <t>3309.31</t>
-  </si>
-  <si>
-    <t>1309.43</t>
-  </si>
-  <si>
-    <t>1915878</t>
-  </si>
-  <si>
-    <t>7546</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>7567.7</t>
-  </si>
-  <si>
-    <t>655.2</t>
-  </si>
-  <si>
-    <t>147.6</t>
-  </si>
-  <si>
-    <t>174.3</t>
-  </si>
-  <si>
-    <t>401.94</t>
-  </si>
-  <si>
-    <t>9795.57</t>
-  </si>
-  <si>
-    <t>919.87</t>
-  </si>
-  <si>
-    <t>8030.4</t>
   </si>
 </sst>
 </file>
@@ -623,13 +623,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>307</v>
+        <v>78</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2">
-        <v>1617.46</v>
+        <v>7567.7</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
@@ -640,13 +640,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2">
-        <v>16.04</v>
+        <v>440.44</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -657,13 +657,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>38</v>
+        <v>287</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>440.44</v>
+        <v>1332.8</v>
       </c>
       <c r="E4" t="s">
         <v>50</v>
@@ -674,13 +674,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>287</v>
+        <v>43</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>1332.8</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -691,13 +691,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
-        <v>387.56</v>
+        <v>16.04</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -708,13 +708,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>35</v>
+        <v>900</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="2">
-        <v>73248</v>
+        <v>1915878</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -725,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>347830</v>
+        <v>174.3</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -742,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>23</v>
+        <v>494</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="2">
-        <v>1718.21</v>
+        <v>9795.57</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
@@ -759,13 +759,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>22</v>
+        <v>746</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="2">
-        <v>440.16</v>
+        <v>3309.31</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -776,13 +776,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>746</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>3309.31</v>
+        <v>401.94</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -793,13 +793,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>400</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>1309.43</v>
+        <v>440.16</v>
       </c>
       <c r="E12" t="s">
         <v>58</v>
@@ -810,13 +810,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>900</v>
+        <v>400</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>1915878</v>
+        <v>1309.43</v>
       </c>
       <c r="E13" t="s">
         <v>59</v>
@@ -827,13 +827,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>7546</v>
+        <v>919.87</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
@@ -844,13 +844,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>112</v>
+        <v>7546</v>
       </c>
       <c r="E15" t="s">
         <v>61</v>
@@ -861,13 +861,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>7567.7</v>
+        <v>347830</v>
       </c>
       <c r="E16" t="s">
         <v>62</v>
@@ -878,13 +878,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="2">
-        <v>655.2</v>
+        <v>73248</v>
       </c>
       <c r="E17" t="s">
         <v>63</v>
@@ -895,13 +895,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="2">
-        <v>147.6</v>
+        <v>1718.21</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -912,13 +912,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>21</v>
+        <v>1415</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2">
-        <v>174.3</v>
+        <v>8030.4</v>
       </c>
       <c r="E19" t="s">
         <v>65</v>
@@ -929,13 +929,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2">
-        <v>401.94</v>
+        <v>387.56</v>
       </c>
       <c r="E20" t="s">
         <v>66</v>
@@ -946,13 +946,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>494</v>
+        <v>26</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2">
-        <v>9795.57</v>
+        <v>655.2</v>
       </c>
       <c r="E21" t="s">
         <v>67</v>
@@ -963,13 +963,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2">
-        <v>919.87</v>
+        <v>147.6</v>
       </c>
       <c r="E22" t="s">
         <v>68</v>
@@ -980,13 +980,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="2">
-        <v>1415</v>
+        <v>307</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D23" s="2">
-        <v>8030.4</v>
+        <v>1617.46</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
fixed bibliotheca sql write error
</commit_message>
<xml_diff>
--- a/apple_finrep/output.xlsx
+++ b/apple_finrep/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="8">
   <si>
     <t>file</t>
   </si>
@@ -31,199 +31,13 @@
     <t>built_in_total</t>
   </si>
   <si>
-    <t>87811004_1121_MX</t>
-  </si>
-  <si>
-    <t>87811004_1121_BR</t>
-  </si>
-  <si>
-    <t>87811004_1121_CA</t>
-  </si>
-  <si>
-    <t>87811004_1121_LL</t>
-  </si>
-  <si>
-    <t>87811004_1121_BG</t>
-  </si>
-  <si>
-    <t>87811004_1121_HU</t>
-  </si>
-  <si>
-    <t>87811004_1121_PE</t>
-  </si>
-  <si>
-    <t>87811004_1121_RO</t>
-  </si>
-  <si>
-    <t>87811004_1121_EU</t>
-  </si>
-  <si>
-    <t>87811004_1121_PL</t>
-  </si>
-  <si>
-    <t>87811004_1121_DK</t>
-  </si>
-  <si>
     <t>87811004_1121_GB</t>
-  </si>
-  <si>
-    <t>87811004_1121_SE</t>
-  </si>
-  <si>
-    <t>87811004_1121_JP</t>
-  </si>
-  <si>
-    <t>87811004_1121_CO</t>
-  </si>
-  <si>
-    <t>87811004_1121_CL</t>
-  </si>
-  <si>
-    <t>87811004_1121_CZ</t>
-  </si>
-  <si>
-    <t>87811004_1121_US</t>
-  </si>
-  <si>
-    <t>87811004_1121_CH</t>
-  </si>
-  <si>
-    <t>87811004_1121_NO</t>
-  </si>
-  <si>
-    <t>87811004_1121_NZ</t>
-  </si>
-  <si>
-    <t>87811004_1121_AU</t>
-  </si>
-  <si>
-    <t>MXN</t>
-  </si>
-  <si>
-    <t>BRL</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>BGN</t>
-  </si>
-  <si>
-    <t>HUF</t>
-  </si>
-  <si>
-    <t>PEN</t>
-  </si>
-  <si>
-    <t>RON</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>DKK</t>
   </si>
   <si>
     <t>GBP</t>
   </si>
   <si>
-    <t>SEK</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>CZK</t>
-  </si>
-  <si>
-    <t>CHF</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>AUD</t>
-  </si>
-  <si>
-    <t>7567.7</t>
-  </si>
-  <si>
-    <t>440.44</t>
-  </si>
-  <si>
-    <t>1332.8</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>16.04</t>
-  </si>
-  <si>
-    <t>1915878</t>
-  </si>
-  <si>
-    <t>174.3</t>
-  </si>
-  <si>
-    <t>9795.57</t>
-  </si>
-  <si>
-    <t>3309.31</t>
-  </si>
-  <si>
-    <t>401.94</t>
-  </si>
-  <si>
-    <t>440.16</t>
-  </si>
-  <si>
     <t>1309.43</t>
-  </si>
-  <si>
-    <t>919.87</t>
-  </si>
-  <si>
-    <t>7546</t>
-  </si>
-  <si>
-    <t>347830</t>
-  </si>
-  <si>
-    <t>73248</t>
-  </si>
-  <si>
-    <t>1718.21</t>
-  </si>
-  <si>
-    <t>8030.4</t>
-  </si>
-  <si>
-    <t>387.56</t>
-  </si>
-  <si>
-    <t>655.2</t>
-  </si>
-  <si>
-    <t>147.6</t>
-  </si>
-  <si>
-    <t>1617.46</t>
   </si>
 </sst>
 </file>
@@ -595,9 +409,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -623,373 +437,373 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>78</v>
+        <v>400</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>7567.7</v>
+        <v>1309.43</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>38</v>
+        <v>400</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2">
-        <v>440.44</v>
+        <v>1309.43</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>287</v>
+        <v>400</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>1332.8</v>
+        <v>1309.43</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>43</v>
+        <v>400</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
-        <v>112</v>
+        <v>1309.43</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>6</v>
+        <v>400</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>16.04</v>
+        <v>1309.43</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>900</v>
+        <v>400</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2">
-        <v>1915878</v>
+        <v>1309.43</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>21</v>
+        <v>400</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2">
-        <v>174.3</v>
+        <v>1309.43</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>494</v>
+        <v>400</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2">
-        <v>9795.57</v>
+        <v>1309.43</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
-        <v>746</v>
+        <v>400</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2">
-        <v>3309.31</v>
+        <v>1309.43</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
-        <v>42</v>
+        <v>400</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2">
-        <v>401.94</v>
+        <v>1309.43</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
-        <v>22</v>
+        <v>400</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D12" s="2">
-        <v>440.16</v>
+        <v>1309.43</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>400</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2">
         <v>1309.43</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2">
-        <v>36</v>
+        <v>400</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>919.87</v>
+        <v>1309.43</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
-        <v>23</v>
+        <v>400</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2">
-        <v>7546</v>
+        <v>1309.43</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
-        <v>31</v>
+        <v>400</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2">
-        <v>347830</v>
+        <v>1309.43</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2">
-        <v>35</v>
+        <v>400</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2">
-        <v>73248</v>
+        <v>1309.43</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>23</v>
+        <v>400</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2">
-        <v>1718.21</v>
+        <v>1309.43</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
-        <v>1415</v>
+        <v>400</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2">
-        <v>8030.4</v>
+        <v>1309.43</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>78</v>
+        <v>400</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2">
-        <v>387.56</v>
+        <v>1309.43</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>26</v>
+        <v>400</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>655.2</v>
+        <v>1309.43</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
-        <v>34</v>
+        <v>400</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D22" s="2">
-        <v>147.6</v>
+        <v>1309.43</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2">
-        <v>307</v>
+        <v>400</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D23" s="2">
-        <v>1617.46</v>
+        <v>1309.43</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
standardize structures of writers
</commit_message>
<xml_diff>
--- a/apple_finrep/output.xlsx
+++ b/apple_finrep/output.xlsx
@@ -31,199 +31,199 @@
     <t>built_in_total</t>
   </si>
   <si>
-    <t>87811004_1121_MX</t>
-  </si>
-  <si>
-    <t>87811004_1121_BR</t>
-  </si>
-  <si>
-    <t>87811004_1121_CA</t>
-  </si>
-  <si>
-    <t>87811004_1121_LL</t>
-  </si>
-  <si>
-    <t>87811004_1121_BG</t>
-  </si>
-  <si>
-    <t>87811004_1121_HU</t>
-  </si>
-  <si>
-    <t>87811004_1121_PE</t>
-  </si>
-  <si>
-    <t>87811004_1121_RO</t>
-  </si>
-  <si>
-    <t>87811004_1121_EU</t>
-  </si>
-  <si>
-    <t>87811004_1121_PL</t>
-  </si>
-  <si>
-    <t>87811004_1121_DK</t>
-  </si>
-  <si>
-    <t>87811004_1121_GB</t>
-  </si>
-  <si>
-    <t>87811004_1121_SE</t>
-  </si>
-  <si>
-    <t>87811004_1121_JP</t>
-  </si>
-  <si>
-    <t>87811004_1121_CO</t>
-  </si>
-  <si>
-    <t>87811004_1121_CL</t>
-  </si>
-  <si>
-    <t>87811004_1121_CZ</t>
-  </si>
-  <si>
-    <t>87811004_1121_US</t>
-  </si>
-  <si>
-    <t>87811004_1121_CH</t>
-  </si>
-  <si>
-    <t>87811004_1121_NO</t>
-  </si>
-  <si>
-    <t>87811004_1121_NZ</t>
-  </si>
-  <si>
-    <t>87811004_1121_AU</t>
+    <t>87811004_0222_RO</t>
+  </si>
+  <si>
+    <t>87811004_0222_PE</t>
+  </si>
+  <si>
+    <t>87811004_0222_HU</t>
+  </si>
+  <si>
+    <t>87811004_0222_EU</t>
+  </si>
+  <si>
+    <t>87811004_0222_MX</t>
+  </si>
+  <si>
+    <t>87811004_0222_LL</t>
+  </si>
+  <si>
+    <t>87811004_0222_BG</t>
+  </si>
+  <si>
+    <t>87811004_0222_BR</t>
+  </si>
+  <si>
+    <t>87811004_0222_CA</t>
+  </si>
+  <si>
+    <t>87811004_0222_CZ</t>
+  </si>
+  <si>
+    <t>87811004_0222_CL</t>
+  </si>
+  <si>
+    <t>87811004_0222_CO</t>
+  </si>
+  <si>
+    <t>87811004_0222_NZ</t>
+  </si>
+  <si>
+    <t>87811004_0222_AU</t>
+  </si>
+  <si>
+    <t>87811004_0222_CH</t>
+  </si>
+  <si>
+    <t>87811004_0222_NO</t>
+  </si>
+  <si>
+    <t>87811004_0222_US</t>
+  </si>
+  <si>
+    <t>87811004_0222_DK</t>
+  </si>
+  <si>
+    <t>87811004_0222_PL</t>
+  </si>
+  <si>
+    <t>87811004_0222_SE</t>
+  </si>
+  <si>
+    <t>87811004_0222_JP</t>
+  </si>
+  <si>
+    <t>87811004_0222_GB</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
   <si>
     <t>MXN</t>
   </si>
   <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
     <t>BRL</t>
   </si>
   <si>
     <t>CAD</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>BGN</t>
-  </si>
-  <si>
-    <t>HUF</t>
-  </si>
-  <si>
-    <t>PEN</t>
-  </si>
-  <si>
-    <t>RON</t>
-  </si>
-  <si>
-    <t>EUR</t>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>NZD</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>DKK</t>
   </si>
   <si>
     <t>PLN</t>
   </si>
   <si>
-    <t>DKK</t>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>JPY</t>
   </si>
   <si>
     <t>GBP</t>
   </si>
   <si>
-    <t>SEK</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>CZK</t>
-  </si>
-  <si>
-    <t>CHF</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>AUD</t>
-  </si>
-  <si>
-    <t>7567.7</t>
-  </si>
-  <si>
-    <t>440.44</t>
-  </si>
-  <si>
-    <t>1332.8</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>16.04</t>
-  </si>
-  <si>
-    <t>1915878</t>
-  </si>
-  <si>
-    <t>174.3</t>
-  </si>
-  <si>
-    <t>9795.57</t>
-  </si>
-  <si>
-    <t>3309.31</t>
-  </si>
-  <si>
-    <t>401.94</t>
-  </si>
-  <si>
-    <t>440.16</t>
-  </si>
-  <si>
-    <t>1309.43</t>
-  </si>
-  <si>
-    <t>919.87</t>
-  </si>
-  <si>
-    <t>7546</t>
-  </si>
-  <si>
-    <t>347830</t>
-  </si>
-  <si>
-    <t>73248</t>
-  </si>
-  <si>
-    <t>1718.21</t>
-  </si>
-  <si>
-    <t>8030.4</t>
-  </si>
-  <si>
-    <t>387.56</t>
-  </si>
-  <si>
-    <t>655.2</t>
-  </si>
-  <si>
-    <t>147.6</t>
-  </si>
-  <si>
-    <t>1617.46</t>
+    <t>10192.91</t>
+  </si>
+  <si>
+    <t>169.05</t>
+  </si>
+  <si>
+    <t>2197785</t>
+  </si>
+  <si>
+    <t>4280.03</t>
+  </si>
+  <si>
+    <t>5686.8</t>
+  </si>
+  <si>
+    <t>100.1</t>
+  </si>
+  <si>
+    <t>12.18</t>
+  </si>
+  <si>
+    <t>678.02</t>
+  </si>
+  <si>
+    <t>1720.6</t>
+  </si>
+  <si>
+    <t>1162</t>
+  </si>
+  <si>
+    <t>43805</t>
+  </si>
+  <si>
+    <t>183120</t>
+  </si>
+  <si>
+    <t>217.42</t>
+  </si>
+  <si>
+    <t>2286.56</t>
+  </si>
+  <si>
+    <t>281.01</t>
+  </si>
+  <si>
+    <t>887.6</t>
+  </si>
+  <si>
+    <t>11197.9</t>
+  </si>
+  <si>
+    <t>478.8</t>
+  </si>
+  <si>
+    <t>498.12</t>
+  </si>
+  <si>
+    <t>1740.73</t>
+  </si>
+  <si>
+    <t>11340</t>
+  </si>
+  <si>
+    <t>1597.17</t>
   </si>
 </sst>
 </file>
@@ -623,13 +623,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>78</v>
+        <v>447</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2">
-        <v>7567.7</v>
+        <v>10192.91</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
@@ -640,13 +640,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2">
-        <v>440.44</v>
+        <v>169.05</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -657,13 +657,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>287</v>
+        <v>1032</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>1332.8</v>
+        <v>2197785</v>
       </c>
       <c r="E4" t="s">
         <v>50</v>
@@ -674,13 +674,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>43</v>
+        <v>790</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>112</v>
+        <v>4280.03</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -691,13 +691,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
-        <v>16.04</v>
+        <v>5686.8</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -708,13 +708,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>900</v>
+        <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="2">
-        <v>1915878</v>
+        <v>100.1</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -725,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>174.3</v>
+        <v>12.18</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -742,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>494</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="2">
-        <v>9795.57</v>
+        <v>678.02</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
@@ -759,13 +759,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>746</v>
+        <v>333</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="2">
-        <v>3309.31</v>
+        <v>1720.6</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -776,13 +776,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>401.94</v>
+        <v>1162</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -793,13 +793,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>440.16</v>
+        <v>43805</v>
       </c>
       <c r="E12" t="s">
         <v>58</v>
@@ -810,13 +810,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>400</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>1309.43</v>
+        <v>183120</v>
       </c>
       <c r="E13" t="s">
         <v>59</v>
@@ -827,13 +827,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>919.87</v>
+        <v>217.42</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
@@ -844,13 +844,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>23</v>
+        <v>357</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>7546</v>
+        <v>2286.56</v>
       </c>
       <c r="E15" t="s">
         <v>61</v>
@@ -861,13 +861,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>347830</v>
+        <v>281.01</v>
       </c>
       <c r="E16" t="s">
         <v>62</v>
@@ -878,13 +878,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="2">
-        <v>73248</v>
+        <v>887.6</v>
       </c>
       <c r="E17" t="s">
         <v>63</v>
@@ -895,13 +895,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>23</v>
+        <v>1575</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2">
-        <v>1718.21</v>
+        <v>11197.9</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -912,13 +912,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>1415</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2">
-        <v>8030.4</v>
+        <v>478.8</v>
       </c>
       <c r="E19" t="s">
         <v>65</v>
@@ -929,13 +929,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="2">
-        <v>387.56</v>
+        <v>498.12</v>
       </c>
       <c r="E20" t="s">
         <v>66</v>
@@ -946,13 +946,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="2">
-        <v>655.2</v>
+        <v>1740.73</v>
       </c>
       <c r="E21" t="s">
         <v>67</v>
@@ -963,13 +963,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D22" s="2">
-        <v>147.6</v>
+        <v>11340</v>
       </c>
       <c r="E22" t="s">
         <v>68</v>
@@ -980,13 +980,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="2">
-        <v>307</v>
+        <v>453</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="2">
-        <v>1617.46</v>
+        <v>1597.17</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
amazo and apple re-arranged
</commit_message>
<xml_diff>
--- a/apple_finrep/output.xlsx
+++ b/apple_finrep/output.xlsx
@@ -31,199 +31,199 @@
     <t>built_in_total</t>
   </si>
   <si>
-    <t>87811004_0222_AU</t>
-  </si>
-  <si>
-    <t>87811004_0222_BG</t>
-  </si>
-  <si>
-    <t>87811004_0222_BR</t>
-  </si>
-  <si>
-    <t>87811004_0222_CA</t>
-  </si>
-  <si>
-    <t>87811004_0222_CH</t>
-  </si>
-  <si>
-    <t>87811004_0222_CL</t>
-  </si>
-  <si>
-    <t>87811004_0222_CO</t>
-  </si>
-  <si>
-    <t>87811004_0222_CZ</t>
-  </si>
-  <si>
-    <t>87811004_0222_DK</t>
-  </si>
-  <si>
-    <t>87811004_0222_EU</t>
-  </si>
-  <si>
-    <t>87811004_0222_GB</t>
-  </si>
-  <si>
-    <t>87811004_0222_HU</t>
-  </si>
-  <si>
-    <t>87811004_0222_JP</t>
-  </si>
-  <si>
-    <t>87811004_0222_LL</t>
-  </si>
-  <si>
-    <t>87811004_0222_MX</t>
-  </si>
-  <si>
-    <t>87811004_0222_NO</t>
-  </si>
-  <si>
-    <t>87811004_0222_NZ</t>
-  </si>
-  <si>
-    <t>87811004_0222_PE</t>
-  </si>
-  <si>
-    <t>87811004_0222_PL</t>
-  </si>
-  <si>
-    <t>87811004_0222_RO</t>
-  </si>
-  <si>
-    <t>87811004_0222_SE</t>
-  </si>
-  <si>
-    <t>87811004_0222_US</t>
+    <t>87811004_0322_RO</t>
+  </si>
+  <si>
+    <t>87811004_0322_PE</t>
+  </si>
+  <si>
+    <t>87811004_0322_HU</t>
+  </si>
+  <si>
+    <t>87811004_0322_EU</t>
+  </si>
+  <si>
+    <t>87811004_0322_MX</t>
+  </si>
+  <si>
+    <t>87811004_0322_LL</t>
+  </si>
+  <si>
+    <t>87811004_0322_BG</t>
+  </si>
+  <si>
+    <t>87811004_0322_BR</t>
+  </si>
+  <si>
+    <t>87811004_0322_CA</t>
+  </si>
+  <si>
+    <t>87811004_0322_CZ</t>
+  </si>
+  <si>
+    <t>87811004_0322_CL</t>
+  </si>
+  <si>
+    <t>87811004_0322_CO</t>
+  </si>
+  <si>
+    <t>87811004_0322_NZ</t>
+  </si>
+  <si>
+    <t>87811004_0322_AU</t>
+  </si>
+  <si>
+    <t>87811004_0322_CH</t>
+  </si>
+  <si>
+    <t>87811004_0322_NO</t>
+  </si>
+  <si>
+    <t>87811004_0322_US</t>
+  </si>
+  <si>
+    <t>87811004_0322_DK</t>
+  </si>
+  <si>
+    <t>87811004_0322_PL</t>
+  </si>
+  <si>
+    <t>87811004_0322_SE</t>
+  </si>
+  <si>
+    <t>87811004_0322_JP</t>
+  </si>
+  <si>
+    <t>87811004_0322_GB</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>NZD</t>
   </si>
   <si>
     <t>AUD</t>
   </si>
   <si>
-    <t>BGN</t>
-  </si>
-  <si>
-    <t>BRL</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
     <t>CHF</t>
   </si>
   <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>CZK</t>
+    <t>NOK</t>
   </si>
   <si>
     <t>DKK</t>
   </si>
   <si>
-    <t>EUR</t>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>JPY</t>
   </si>
   <si>
     <t>GBP</t>
   </si>
   <si>
-    <t>HUF</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>MXN</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>PEN</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>RON</t>
-  </si>
-  <si>
-    <t>SEK</t>
-  </si>
-  <si>
-    <t>2286.56</t>
-  </si>
-  <si>
-    <t>12.18</t>
-  </si>
-  <si>
-    <t>678.02</t>
-  </si>
-  <si>
-    <t>1720.6</t>
-  </si>
-  <si>
-    <t>281.01</t>
-  </si>
-  <si>
-    <t>43805</t>
-  </si>
-  <si>
-    <t>183120</t>
-  </si>
-  <si>
-    <t>1162</t>
-  </si>
-  <si>
-    <t>478.8</t>
-  </si>
-  <si>
-    <t>4280.03</t>
-  </si>
-  <si>
-    <t>1597.17</t>
-  </si>
-  <si>
-    <t>2197785</t>
-  </si>
-  <si>
-    <t>11340</t>
-  </si>
-  <si>
-    <t>100.1</t>
-  </si>
-  <si>
-    <t>5686.8</t>
-  </si>
-  <si>
-    <t>887.6</t>
-  </si>
-  <si>
-    <t>217.42</t>
-  </si>
-  <si>
-    <t>169.05</t>
-  </si>
-  <si>
-    <t>498.12</t>
-  </si>
-  <si>
-    <t>10192.91</t>
-  </si>
-  <si>
-    <t>1740.73</t>
-  </si>
-  <si>
-    <t>11197.9</t>
+    <t>9983.42</t>
+  </si>
+  <si>
+    <t>141.96</t>
+  </si>
+  <si>
+    <t>1882603</t>
+  </si>
+  <si>
+    <t>3090.3</t>
+  </si>
+  <si>
+    <t>4825.1</t>
+  </si>
+  <si>
+    <t>96.6</t>
+  </si>
+  <si>
+    <t>22.44</t>
+  </si>
+  <si>
+    <t>334.81</t>
+  </si>
+  <si>
+    <t>1753.5</t>
+  </si>
+  <si>
+    <t>636.36</t>
+  </si>
+  <si>
+    <t>63087</t>
+  </si>
+  <si>
+    <t>286230</t>
+  </si>
+  <si>
+    <t>208.33</t>
+  </si>
+  <si>
+    <t>3178.64</t>
+  </si>
+  <si>
+    <t>243.39</t>
+  </si>
+  <si>
+    <t>682.5</t>
+  </si>
+  <si>
+    <t>10299.1</t>
+  </si>
+  <si>
+    <t>268.24</t>
+  </si>
+  <si>
+    <t>517.94</t>
+  </si>
+  <si>
+    <t>931.77</t>
+  </si>
+  <si>
+    <t>5950</t>
+  </si>
+  <si>
+    <t>1593.33</t>
   </si>
 </sst>
 </file>
@@ -623,13 +623,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>357</v>
+        <v>423</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2">
-        <v>2286.56</v>
+        <v>9983.42</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
@@ -640,13 +640,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2">
-        <v>12.18</v>
+        <v>141.96</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -657,13 +657,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>41</v>
+        <v>954</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>678.02</v>
+        <v>1882603</v>
       </c>
       <c r="E4" t="s">
         <v>50</v>
@@ -674,13 +674,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>333</v>
+        <v>716</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>1720.6</v>
+        <v>3090.3</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -691,13 +691,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
-        <v>281.01</v>
+        <v>4825.1</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -708,13 +708,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="2">
-        <v>43805</v>
+        <v>96.59999999999999</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -725,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>183120</v>
+        <v>22.44</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -742,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="2">
-        <v>1162</v>
+        <v>334.81</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
@@ -759,13 +759,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>31</v>
+        <v>324</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="2">
-        <v>478.8</v>
+        <v>1753.5</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -776,13 +776,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>790</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>4280.03</v>
+        <v>636.36</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -793,13 +793,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>453</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>1597.17</v>
+        <v>63087</v>
       </c>
       <c r="E12" t="s">
         <v>58</v>
@@ -810,13 +810,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>1032</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>2197785</v>
+        <v>286230</v>
       </c>
       <c r="E13" t="s">
         <v>59</v>
@@ -827,13 +827,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>11340</v>
+        <v>208.33</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
@@ -844,13 +844,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>38</v>
+        <v>367</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>100.1</v>
+        <v>3178.64</v>
       </c>
       <c r="E15" t="s">
         <v>61</v>
@@ -861,13 +861,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>5686.8</v>
+        <v>243.39</v>
       </c>
       <c r="E16" t="s">
         <v>62</v>
@@ -878,13 +878,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="2">
-        <v>887.6</v>
+        <v>682.5</v>
       </c>
       <c r="E17" t="s">
         <v>63</v>
@@ -895,13 +895,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>58</v>
+        <v>1487</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2">
-        <v>217.42</v>
+        <v>10299.1</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -912,13 +912,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2">
-        <v>169.05</v>
+        <v>268.24</v>
       </c>
       <c r="E19" t="s">
         <v>65</v>
@@ -929,13 +929,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
+        <v>46</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D20" s="2">
-        <v>498.12</v>
+        <v>517.9400000000001</v>
       </c>
       <c r="E20" t="s">
         <v>66</v>
@@ -946,13 +946,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>447</v>
+        <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2">
-        <v>10192.91</v>
+        <v>931.77</v>
       </c>
       <c r="E21" t="s">
         <v>67</v>
@@ -963,13 +963,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2">
-        <v>1740.73</v>
+        <v>5950</v>
       </c>
       <c r="E22" t="s">
         <v>68</v>
@@ -980,13 +980,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="2">
-        <v>1575</v>
+        <v>477</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D23" s="2">
-        <v>11197.9</v>
+        <v>1593.33</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
datacamp.log not to git it | gitignore update
</commit_message>
<xml_diff>
--- a/apple_finrep/output.xlsx
+++ b/apple_finrep/output.xlsx
@@ -31,199 +31,199 @@
     <t>built_in_total</t>
   </si>
   <si>
+    <t>87811004_0322_AU</t>
+  </si>
+  <si>
+    <t>87811004_0322_BG</t>
+  </si>
+  <si>
+    <t>87811004_0322_BR</t>
+  </si>
+  <si>
+    <t>87811004_0322_CA</t>
+  </si>
+  <si>
+    <t>87811004_0322_CH</t>
+  </si>
+  <si>
+    <t>87811004_0322_CL</t>
+  </si>
+  <si>
+    <t>87811004_0322_CO</t>
+  </si>
+  <si>
+    <t>87811004_0322_CZ</t>
+  </si>
+  <si>
+    <t>87811004_0322_DK</t>
+  </si>
+  <si>
+    <t>87811004_0322_EU</t>
+  </si>
+  <si>
+    <t>87811004_0322_GB</t>
+  </si>
+  <si>
+    <t>87811004_0322_HU</t>
+  </si>
+  <si>
+    <t>87811004_0322_JP</t>
+  </si>
+  <si>
+    <t>87811004_0322_LL</t>
+  </si>
+  <si>
+    <t>87811004_0322_MX</t>
+  </si>
+  <si>
+    <t>87811004_0322_NO</t>
+  </si>
+  <si>
+    <t>87811004_0322_NZ</t>
+  </si>
+  <si>
+    <t>87811004_0322_PE</t>
+  </si>
+  <si>
+    <t>87811004_0322_PL</t>
+  </si>
+  <si>
     <t>87811004_0322_RO</t>
   </si>
   <si>
-    <t>87811004_0322_PE</t>
-  </si>
-  <si>
-    <t>87811004_0322_HU</t>
-  </si>
-  <si>
-    <t>87811004_0322_EU</t>
-  </si>
-  <si>
-    <t>87811004_0322_MX</t>
-  </si>
-  <si>
-    <t>87811004_0322_LL</t>
-  </si>
-  <si>
-    <t>87811004_0322_BG</t>
-  </si>
-  <si>
-    <t>87811004_0322_BR</t>
-  </si>
-  <si>
-    <t>87811004_0322_CA</t>
-  </si>
-  <si>
-    <t>87811004_0322_CZ</t>
-  </si>
-  <si>
-    <t>87811004_0322_CL</t>
-  </si>
-  <si>
-    <t>87811004_0322_CO</t>
-  </si>
-  <si>
-    <t>87811004_0322_NZ</t>
-  </si>
-  <si>
-    <t>87811004_0322_AU</t>
-  </si>
-  <si>
-    <t>87811004_0322_CH</t>
-  </si>
-  <si>
-    <t>87811004_0322_NO</t>
+    <t>87811004_0322_SE</t>
   </si>
   <si>
     <t>87811004_0322_US</t>
   </si>
   <si>
-    <t>87811004_0322_DK</t>
-  </si>
-  <si>
-    <t>87811004_0322_PL</t>
-  </si>
-  <si>
-    <t>87811004_0322_SE</t>
-  </si>
-  <si>
-    <t>87811004_0322_JP</t>
-  </si>
-  <si>
-    <t>87811004_0322_GB</t>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>NZD</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>PLN</t>
   </si>
   <si>
     <t>RON</t>
   </si>
   <si>
-    <t>PEN</t>
-  </si>
-  <si>
-    <t>HUF</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>MXN</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>BGN</t>
-  </si>
-  <si>
-    <t>BRL</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>CZK</t>
-  </si>
-  <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>AUD</t>
-  </si>
-  <si>
-    <t>CHF</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>DKK</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
     <t>SEK</t>
   </si>
   <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>GBP</t>
+    <t>3178.64</t>
+  </si>
+  <si>
+    <t>22.44</t>
+  </si>
+  <si>
+    <t>334.81</t>
+  </si>
+  <si>
+    <t>1753.5</t>
+  </si>
+  <si>
+    <t>243.39</t>
+  </si>
+  <si>
+    <t>63087</t>
+  </si>
+  <si>
+    <t>286230</t>
+  </si>
+  <si>
+    <t>636.36</t>
+  </si>
+  <si>
+    <t>268.24</t>
+  </si>
+  <si>
+    <t>3090.3</t>
+  </si>
+  <si>
+    <t>1593.33</t>
+  </si>
+  <si>
+    <t>1882603</t>
+  </si>
+  <si>
+    <t>5950</t>
+  </si>
+  <si>
+    <t>96.6</t>
+  </si>
+  <si>
+    <t>4825.1</t>
+  </si>
+  <si>
+    <t>682.5</t>
+  </si>
+  <si>
+    <t>208.33</t>
+  </si>
+  <si>
+    <t>141.96</t>
+  </si>
+  <si>
+    <t>517.94</t>
   </si>
   <si>
     <t>9983.42</t>
   </si>
   <si>
-    <t>141.96</t>
-  </si>
-  <si>
-    <t>1882603</t>
-  </si>
-  <si>
-    <t>3090.3</t>
-  </si>
-  <si>
-    <t>4825.1</t>
-  </si>
-  <si>
-    <t>96.6</t>
-  </si>
-  <si>
-    <t>22.44</t>
-  </si>
-  <si>
-    <t>334.81</t>
-  </si>
-  <si>
-    <t>1753.5</t>
-  </si>
-  <si>
-    <t>636.36</t>
-  </si>
-  <si>
-    <t>63087</t>
-  </si>
-  <si>
-    <t>286230</t>
-  </si>
-  <si>
-    <t>208.33</t>
-  </si>
-  <si>
-    <t>3178.64</t>
-  </si>
-  <si>
-    <t>243.39</t>
-  </si>
-  <si>
-    <t>682.5</t>
+    <t>931.77</t>
   </si>
   <si>
     <t>10299.1</t>
-  </si>
-  <si>
-    <t>268.24</t>
-  </si>
-  <si>
-    <t>517.94</t>
-  </si>
-  <si>
-    <t>931.77</t>
-  </si>
-  <si>
-    <t>5950</t>
-  </si>
-  <si>
-    <t>1593.33</t>
   </si>
 </sst>
 </file>
@@ -623,13 +623,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>423</v>
+        <v>367</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2">
-        <v>9983.42</v>
+        <v>3178.64</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
@@ -640,13 +640,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2">
-        <v>141.96</v>
+        <v>22.44</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -657,13 +657,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>954</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>1882603</v>
+        <v>334.81</v>
       </c>
       <c r="E4" t="s">
         <v>50</v>
@@ -674,13 +674,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>716</v>
+        <v>324</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>3090.3</v>
+        <v>1753.5</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -691,13 +691,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
-        <v>4825.1</v>
+        <v>243.39</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -708,13 +708,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="2">
-        <v>96.59999999999999</v>
+        <v>63087</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -725,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>22.44</v>
+        <v>286230</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -742,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="2">
-        <v>334.81</v>
+        <v>636.36</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
@@ -759,13 +759,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>324</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="2">
-        <v>1753.5</v>
+        <v>268.24</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -776,13 +776,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>12</v>
+        <v>716</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>636.36</v>
+        <v>3090.3</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -793,13 +793,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>31</v>
+        <v>477</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>63087</v>
+        <v>1593.33</v>
       </c>
       <c r="E12" t="s">
         <v>58</v>
@@ -810,13 +810,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>31</v>
+        <v>954</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>286230</v>
+        <v>1882603</v>
       </c>
       <c r="E13" t="s">
         <v>59</v>
@@ -827,13 +827,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>208.33</v>
+        <v>5950</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
@@ -844,13 +844,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>367</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>3178.64</v>
+        <v>96.59999999999999</v>
       </c>
       <c r="E15" t="s">
         <v>61</v>
@@ -861,13 +861,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>243.39</v>
+        <v>4825.1</v>
       </c>
       <c r="E16" t="s">
         <v>62</v>
@@ -895,13 +895,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>1487</v>
+        <v>51</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D18" s="2">
-        <v>10299.1</v>
+        <v>208.33</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -912,13 +912,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2">
-        <v>268.24</v>
+        <v>141.96</v>
       </c>
       <c r="E19" t="s">
         <v>65</v>
@@ -932,7 +932,7 @@
         <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2">
         <v>517.9400000000001</v>
@@ -946,13 +946,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>32</v>
+        <v>423</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2">
-        <v>931.77</v>
+        <v>9983.42</v>
       </c>
       <c r="E21" t="s">
         <v>67</v>
@@ -963,13 +963,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2">
-        <v>5950</v>
+        <v>931.77</v>
       </c>
       <c r="E22" t="s">
         <v>68</v>
@@ -980,13 +980,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="2">
-        <v>477</v>
+        <v>1487</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D23" s="2">
-        <v>1593.33</v>
+        <v>10299.1</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
dotenv .env and non-existent check
</commit_message>
<xml_diff>
--- a/apple_finrep/output.xlsx
+++ b/apple_finrep/output.xlsx
@@ -31,199 +31,199 @@
     <t>built_in_total</t>
   </si>
   <si>
+    <t>87811004_0322_RO</t>
+  </si>
+  <si>
+    <t>87811004_0322_PE</t>
+  </si>
+  <si>
+    <t>87811004_0322_HU</t>
+  </si>
+  <si>
+    <t>87811004_0322_EU</t>
+  </si>
+  <si>
+    <t>87811004_0322_MX</t>
+  </si>
+  <si>
+    <t>87811004_0322_LL</t>
+  </si>
+  <si>
+    <t>87811004_0322_BG</t>
+  </si>
+  <si>
+    <t>87811004_0322_BR</t>
+  </si>
+  <si>
+    <t>87811004_0322_CA</t>
+  </si>
+  <si>
+    <t>87811004_0322_CZ</t>
+  </si>
+  <si>
+    <t>87811004_0322_CL</t>
+  </si>
+  <si>
+    <t>87811004_0322_CO</t>
+  </si>
+  <si>
+    <t>87811004_0322_NZ</t>
+  </si>
+  <si>
     <t>87811004_0322_AU</t>
   </si>
   <si>
-    <t>87811004_0322_BG</t>
-  </si>
-  <si>
-    <t>87811004_0322_BR</t>
-  </si>
-  <si>
-    <t>87811004_0322_CA</t>
-  </si>
-  <si>
     <t>87811004_0322_CH</t>
   </si>
   <si>
-    <t>87811004_0322_CL</t>
-  </si>
-  <si>
-    <t>87811004_0322_CO</t>
-  </si>
-  <si>
-    <t>87811004_0322_CZ</t>
+    <t>87811004_0322_NO</t>
+  </si>
+  <si>
+    <t>87811004_0322_US</t>
   </si>
   <si>
     <t>87811004_0322_DK</t>
   </si>
   <si>
-    <t>87811004_0322_EU</t>
+    <t>87811004_0322_PL</t>
+  </si>
+  <si>
+    <t>87811004_0322_SE</t>
+  </si>
+  <si>
+    <t>87811004_0322_JP</t>
   </si>
   <si>
     <t>87811004_0322_GB</t>
   </si>
   <si>
-    <t>87811004_0322_HU</t>
-  </si>
-  <si>
-    <t>87811004_0322_JP</t>
-  </si>
-  <si>
-    <t>87811004_0322_LL</t>
-  </si>
-  <si>
-    <t>87811004_0322_MX</t>
-  </si>
-  <si>
-    <t>87811004_0322_NO</t>
-  </si>
-  <si>
-    <t>87811004_0322_NZ</t>
-  </si>
-  <si>
-    <t>87811004_0322_PE</t>
-  </si>
-  <si>
-    <t>87811004_0322_PL</t>
-  </si>
-  <si>
-    <t>87811004_0322_RO</t>
-  </si>
-  <si>
-    <t>87811004_0322_SE</t>
-  </si>
-  <si>
-    <t>87811004_0322_US</t>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>NZD</t>
   </si>
   <si>
     <t>AUD</t>
   </si>
   <si>
-    <t>BGN</t>
-  </si>
-  <si>
-    <t>BRL</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
     <t>CHF</t>
   </si>
   <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>CZK</t>
+    <t>NOK</t>
   </si>
   <si>
     <t>DKK</t>
   </si>
   <si>
-    <t>EUR</t>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>JPY</t>
   </si>
   <si>
     <t>GBP</t>
   </si>
   <si>
-    <t>HUF</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>MXN</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>PEN</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>RON</t>
-  </si>
-  <si>
-    <t>SEK</t>
+    <t>9983.42</t>
+  </si>
+  <si>
+    <t>141.96</t>
+  </si>
+  <si>
+    <t>1882603</t>
+  </si>
+  <si>
+    <t>3090.3</t>
+  </si>
+  <si>
+    <t>4825.1</t>
+  </si>
+  <si>
+    <t>96.6</t>
+  </si>
+  <si>
+    <t>22.44</t>
+  </si>
+  <si>
+    <t>334.81</t>
+  </si>
+  <si>
+    <t>1753.5</t>
+  </si>
+  <si>
+    <t>636.36</t>
+  </si>
+  <si>
+    <t>63087</t>
+  </si>
+  <si>
+    <t>286230</t>
+  </si>
+  <si>
+    <t>208.33</t>
   </si>
   <si>
     <t>3178.64</t>
   </si>
   <si>
-    <t>22.44</t>
-  </si>
-  <si>
-    <t>334.81</t>
-  </si>
-  <si>
-    <t>1753.5</t>
-  </si>
-  <si>
     <t>243.39</t>
   </si>
   <si>
-    <t>63087</t>
-  </si>
-  <si>
-    <t>286230</t>
-  </si>
-  <si>
-    <t>636.36</t>
+    <t>682.5</t>
+  </si>
+  <si>
+    <t>10299.1</t>
   </si>
   <si>
     <t>268.24</t>
   </si>
   <si>
-    <t>3090.3</t>
+    <t>517.94</t>
+  </si>
+  <si>
+    <t>931.77</t>
+  </si>
+  <si>
+    <t>5950</t>
   </si>
   <si>
     <t>1593.33</t>
-  </si>
-  <si>
-    <t>1882603</t>
-  </si>
-  <si>
-    <t>5950</t>
-  </si>
-  <si>
-    <t>96.6</t>
-  </si>
-  <si>
-    <t>4825.1</t>
-  </si>
-  <si>
-    <t>682.5</t>
-  </si>
-  <si>
-    <t>208.33</t>
-  </si>
-  <si>
-    <t>141.96</t>
-  </si>
-  <si>
-    <t>517.94</t>
-  </si>
-  <si>
-    <t>9983.42</t>
-  </si>
-  <si>
-    <t>931.77</t>
-  </si>
-  <si>
-    <t>10299.1</t>
   </si>
 </sst>
 </file>
@@ -623,13 +623,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>367</v>
+        <v>423</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2">
-        <v>3178.64</v>
+        <v>9983.42</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
@@ -640,13 +640,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2">
-        <v>22.44</v>
+        <v>141.96</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -657,13 +657,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>37</v>
+        <v>954</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>334.81</v>
+        <v>1882603</v>
       </c>
       <c r="E4" t="s">
         <v>50</v>
@@ -674,13 +674,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>324</v>
+        <v>716</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>1753.5</v>
+        <v>3090.3</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -691,13 +691,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
-        <v>243.39</v>
+        <v>4825.1</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
@@ -708,13 +708,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="2">
-        <v>63087</v>
+        <v>96.59999999999999</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -725,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>286230</v>
+        <v>22.44</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -742,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="2">
-        <v>636.36</v>
+        <v>334.81</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
@@ -759,13 +759,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>21</v>
+        <v>324</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="2">
-        <v>268.24</v>
+        <v>1753.5</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -776,13 +776,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>716</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>3090.3</v>
+        <v>636.36</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -793,13 +793,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>477</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>1593.33</v>
+        <v>63087</v>
       </c>
       <c r="E12" t="s">
         <v>58</v>
@@ -810,13 +810,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>954</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>1882603</v>
+        <v>286230</v>
       </c>
       <c r="E13" t="s">
         <v>59</v>
@@ -827,13 +827,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>5950</v>
+        <v>208.33</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
@@ -844,13 +844,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>37</v>
+        <v>367</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>96.59999999999999</v>
+        <v>3178.64</v>
       </c>
       <c r="E15" t="s">
         <v>61</v>
@@ -861,13 +861,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>4825.1</v>
+        <v>243.39</v>
       </c>
       <c r="E16" t="s">
         <v>62</v>
@@ -895,13 +895,13 @@
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>51</v>
+        <v>1487</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2">
-        <v>208.33</v>
+        <v>10299.1</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -912,13 +912,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2">
-        <v>141.96</v>
+        <v>268.24</v>
       </c>
       <c r="E19" t="s">
         <v>65</v>
@@ -932,7 +932,7 @@
         <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2">
         <v>517.9400000000001</v>
@@ -946,13 +946,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>423</v>
+        <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2">
-        <v>9983.42</v>
+        <v>931.77</v>
       </c>
       <c r="E21" t="s">
         <v>67</v>
@@ -963,13 +963,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2">
-        <v>931.77</v>
+        <v>5950</v>
       </c>
       <c r="E22" t="s">
         <v>68</v>
@@ -980,13 +980,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="2">
-        <v>1487</v>
+        <v>477</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D23" s="2">
-        <v>10299.1</v>
+        <v>1593.33</v>
       </c>
       <c r="E23" t="s">
         <v>69</v>

</xml_diff>